<commit_message>
Kanban board screenshot, Google Drive Backup
Kanban board screenshot updated, Google Drive Backup updated
</commit_message>
<xml_diff>
--- a/Team Google Drive Backup/THE PROJECT/Deliverable 1/Deliverable 1 - Sprint Backlog.xlsx
+++ b/Team Google Drive Backup/THE PROJECT/Deliverable 1/Deliverable 1 - Sprint Backlog.xlsx
@@ -98,14 +98,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mh5iHq6vJpRbdDbdomKuvrWRGgc3w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhHp70tybRMu1FJzsswFT9iL22Elg=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -155,7 +155,7 @@
     <t>As a user of this system (student, professor, administrator, etc.) when I encounter a problem, I want to communicate not only the technical details but also how it makes me feel, so that the impact of the problem is fully understood.</t>
   </si>
   <si>
-    <t>Story Tasks Document</t>
+    <t>C1 - Story Document</t>
   </si>
   <si>
     <t>Not Assigned</t>
@@ -176,6 +176,9 @@
     <t>As a feedback provider, I want to track the status of my feedback, so I can understand where it's at in the review process and what actions are being taken.</t>
   </si>
   <si>
+    <t>C2 - Story Document</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
     <t>As a student, I want to connect with others who've shared similar feedback or faced similar issues, so we can collaborate on solutions or offer mutual support.</t>
   </si>
   <si>
+    <t>C3 - Story Document</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
@@ -194,6 +200,9 @@
     <t>As a student, if I have a pressing issue, I want an option to message a specific authority, like a professor or department head, to directly address my concern.</t>
   </si>
   <si>
+    <t>C4 - Story Document</t>
+  </si>
+  <si>
     <t>C5</t>
   </si>
   <si>
@@ -201,6 +210,9 @@
   </si>
   <si>
     <t>As a user (student, professor, administrator, etc.), I want to ask for help anonymously, so that I can alleviate my anxieties and ensure I succeed in the class.</t>
+  </si>
+  <si>
+    <t>C5 - Story Document</t>
   </si>
   <si>
     <t>C6</t>
@@ -807,7 +819,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>17</v>
@@ -832,16 +844,16 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>17</v>
@@ -866,16 +878,16 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>17</v>
@@ -900,16 +912,16 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>17</v>
@@ -934,13 +946,13 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="11" t="s">
@@ -966,13 +978,13 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="11" t="s">
@@ -998,13 +1010,13 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="11" t="s">
@@ -1030,13 +1042,13 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="11" t="s">
@@ -1061,13 +1073,13 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="11" t="s">
@@ -1106,18 +1118,18 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="11" t="s">
@@ -1142,13 +1154,13 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="11" t="s">
@@ -1174,13 +1186,13 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="11" t="s">
@@ -1218,18 +1230,18 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="11" t="s">
@@ -1255,13 +1267,13 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="11" t="s">
@@ -1301,18 +1313,18 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="11" t="s">
@@ -1338,13 +1350,13 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="11" t="s">
@@ -1370,13 +1382,13 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D26" s="24"/>
       <c r="E26" s="11" t="s">

</xml_diff>